<commit_message>
Update migration to ei39
</commit_message>
<xml_diff>
--- a/others/hydrogen market/mapping IAM-IEA.xlsx
+++ b/others/hydrogen market/mapping IAM-IEA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/hydrogen-prospective-scenarios/others/hydrogen market/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/Github/hydrogen-prospective-scenarios/others/hydrogen market/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA65552-49C6-6B44-AC47-76D373893DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D27A1CA-E87E-9A49-BC40-FD0DBA99FDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41500" yWindow="-320" windowWidth="26840" windowHeight="14340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21440" windowHeight="22980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$406</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2409" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2436" uniqueCount="56">
   <si>
     <t>China</t>
   </si>
@@ -189,13 +200,13 @@
     <t>SSP2 - NDC</t>
   </si>
   <si>
-    <t>SSP2 - PkBudg11500</t>
+    <t>Variable</t>
   </si>
   <si>
-    <t>SSP2 - PkBudg500</t>
+    <t>SSP1 - PkBudg500</t>
   </si>
   <si>
-    <t>Variable</t>
+    <t>SSP2 - PkBudg1150</t>
   </si>
 </sst>
 </file>
@@ -548,16 +559,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEF4BDD2-5D39-4ECE-8BF4-156E73BF5FC9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M406"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D285" sqref="D285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27" style="3" customWidth="1"/>
     <col min="3" max="3" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" style="6" bestFit="1" customWidth="1"/>
@@ -582,7 +594,7 @@
         <v>26</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G1" s="1">
         <v>2020</v>
@@ -606,7 +618,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
@@ -647,7 +659,7 @@
         <v>18.570398297093735</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -688,7 +700,7 @@
         <v>0.8412769177613395</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -729,7 +741,7 @@
         <v>6.8651647435611478</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -770,7 +782,7 @@
         <v>0.61896556255770452</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -811,7 +823,7 @@
         <v>2.5799070432606364E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -852,7 +864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -893,7 +905,7 @@
         <v>0.6053828062343003</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -934,7 +946,7 @@
         <v>1.3970372451560775</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -975,7 +987,7 @@
         <v>0.32597535720308479</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1016,7 +1028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
@@ -1057,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
@@ -1098,7 +1110,7 @@
         <v>3.9452371536473168</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
@@ -1139,7 +1151,7 @@
         <v>0.35570390885684039</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1180,7 +1192,7 @@
         <v>5.5321177452031939E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>9</v>
       </c>
@@ -1221,7 +1233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -1262,7 +1274,7 @@
         <v>0.12840824441720258</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1315,7 @@
         <v>0.28535165426045017</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1356,7 @@
         <v>6.1826191756430872E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>9</v>
       </c>
@@ -1467,7 +1479,7 @@
         <v>1.6968259321966528</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>9</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>0.15298639681875945</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
@@ -1549,7 +1561,7 @@
         <v>2.3793350017876293E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>9</v>
       </c>
@@ -1590,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>9</v>
       </c>
@@ -1631,7 +1643,7 @@
         <v>0.14245532990991638</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>9</v>
       </c>
@@ -1672,7 +1684,7 @@
         <v>0.32874306902288392</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>9</v>
       </c>
@@ -1713,7 +1725,7 @@
         <v>7.6706716105339592E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>9</v>
       </c>
@@ -1754,7 +1766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>9</v>
       </c>
@@ -1795,7 +1807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>9</v>
       </c>
@@ -1836,7 +1848,7 @@
         <v>11.821478802327245</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>9</v>
       </c>
@@ -1877,7 +1889,7 @@
         <v>1.0658285052822913</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>9</v>
       </c>
@@ -1918,7 +1930,7 @@
         <v>1.3882731498033606E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -1959,7 +1971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>9</v>
       </c>
@@ -2000,7 +2012,7 @@
         <v>0.86974941543156259</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>9</v>
       </c>
@@ -2041,7 +2053,7 @@
         <v>1.63078015393418</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>9</v>
       </c>
@@ -2082,7 +2094,7 @@
         <v>0.21743735385789065</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -2123,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -2164,7 +2176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
@@ -2205,7 +2217,7 @@
         <v>2.828207485820796</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>9</v>
       </c>
@@ -2246,7 +2258,7 @@
         <v>0.2549921382633733</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>9</v>
       </c>
@@ -2287,7 +2299,7 @@
         <v>3.644380884280778E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>9</v>
       </c>
@@ -2328,7 +2340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>9</v>
       </c>
@@ -2369,7 +2381,7 @@
         <v>0.26009425280805032</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>9</v>
       </c>
@@ -2410,7 +2422,7 @@
         <v>0.45898985789655938</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>9</v>
       </c>
@@ -2451,7 +2463,7 @@
         <v>4.5898985789655941E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>9</v>
       </c>
@@ -2492,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>9</v>
       </c>
@@ -2533,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>9</v>
       </c>
@@ -2574,7 +2586,7 @@
         <v>0.70953989270342366</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>9</v>
       </c>
@@ -2615,7 +2627,7 @@
         <v>6.3972355398494482E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>9</v>
       </c>
@@ -2656,7 +2668,7 @@
         <v>7.4067453223692053E-4</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>9</v>
       </c>
@@ -2697,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>9</v>
       </c>
@@ -2738,7 +2750,7 @@
         <v>3.941090678178634E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>9</v>
       </c>
@@ -2779,7 +2791,7 @@
         <v>9.0948246419506926E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>9</v>
       </c>
@@ -2820,7 +2832,7 @@
         <v>2.1221257497884952E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>9</v>
       </c>
@@ -2861,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>9</v>
       </c>
@@ -2902,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>9</v>
       </c>
@@ -2943,7 +2955,7 @@
         <v>4.0500285910947644</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>9</v>
       </c>
@@ -2984,7 +2996,7 @@
         <v>0.36515194010645086</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>9</v>
       </c>
@@ -3025,7 +3037,7 @@
         <v>4.2277440114408295E-3</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>9</v>
       </c>
@@ -3066,7 +3078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>9</v>
       </c>
@@ -3107,7 +3119,7 @@
         <v>0.24248612438540582</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
@@ -3148,7 +3160,7 @@
         <v>0.42791669009189254</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>9</v>
       </c>
@@ -3189,7 +3201,7 @@
         <v>4.2791669009189258E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>9</v>
       </c>
@@ -3230,7 +3242,7 @@
         <v>0.63419508675853076</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>9</v>
       </c>
@@ -3271,7 +3283,7 @@
         <v>2.873033089070039E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>9</v>
       </c>
@@ -3312,7 +3324,7 @@
         <v>4.8024710694346391</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>9</v>
       </c>
@@ -3353,7 +3365,7 @@
         <v>0.43299240705733777</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>9</v>
       </c>
@@ -3394,7 +3406,7 @@
         <v>5.0405196043379818E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>9</v>
       </c>
@@ -3435,7 +3447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>9</v>
       </c>
@@ -3476,7 +3488,7 @@
         <v>0.13127501909282469</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>9</v>
       </c>
@@ -3517,7 +3529,7 @@
         <v>0.30294235175267231</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>9</v>
       </c>
@@ -3558,7 +3570,7 @@
         <v>6.5118044376803116E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>9</v>
       </c>
@@ -3599,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>9</v>
       </c>
@@ -3640,7 +3652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>9</v>
       </c>
@@ -3681,7 +3693,7 @@
         <v>14.598940270225308</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>9</v>
       </c>
@@ -3722,7 +3734,7 @@
         <v>1.3162453654999968</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>9</v>
       </c>
@@ -3763,7 +3775,7 @@
         <v>1.5239542366821596E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>9</v>
       </c>
@@ -3804,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>9</v>
       </c>
@@ -3845,7 +3857,7 @@
         <v>0.62667500240859975</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>9</v>
       </c>
@@ -3886,7 +3898,7 @@
         <v>1.4461730824813839</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>9</v>
       </c>
@@ -3927,7 +3939,7 @@
         <v>0.33744038591232295</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>9</v>
       </c>
@@ -3968,7 +3980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>9</v>
       </c>
@@ -4009,7 +4021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>9</v>
       </c>
@@ -4050,7 +4062,7 @@
         <v>2.415487316547567</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>9</v>
       </c>
@@ -4091,7 +4103,7 @@
         <v>0.2177811489724446</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>9</v>
       </c>
@@ -4132,7 +4144,7 @@
         <v>5.6304373733762365E-3</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>9</v>
       </c>
@@ -4173,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>9</v>
       </c>
@@ -4214,7 +4226,7 @@
         <v>0.12093351098549149</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>9</v>
       </c>
@@ -4255,7 +4267,7 @@
         <v>0.27907733304344184</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>9</v>
       </c>
@@ -4296,7 +4308,7 @@
         <v>6.5118044376803116E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>9</v>
       </c>
@@ -4337,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>9</v>
       </c>
@@ -4378,7 +4390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -4419,7 +4431,7 @@
         <v>0.23421670420867649</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>9</v>
       </c>
@@ -4460,7 +4472,7 @@
         <v>2.1117056836386126E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>9</v>
       </c>
@@ -4501,7 +4513,7 @@
         <v>5.4403527589083546E-4</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>9</v>
       </c>
@@ -4542,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>9</v>
       </c>
@@ -4583,7 +4595,7 @@
         <v>3.4595595017366622E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>9</v>
       </c>
@@ -4624,7 +4636,7 @@
         <v>7.9835988501615274E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>9</v>
       </c>
@@ -4665,7 +4677,7 @@
         <v>1.8628397317043566E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>9</v>
       </c>
@@ -4706,7 +4718,7 @@
         <v>2.5171004805639003</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>9</v>
       </c>
@@ -4747,7 +4759,7 @@
         <v>0.11402978547400273</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>9</v>
       </c>
@@ -4788,7 +4800,7 @@
         <v>11.166357898444735</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>9</v>
       </c>
@@ -4829,7 +4841,7 @@
         <v>1.0067625842211447</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>9</v>
       </c>
@@ -4870,7 +4882,7 @@
         <v>1.3987605768084855E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>9</v>
       </c>
@@ -4911,7 +4923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>9</v>
       </c>
@@ -4952,7 +4964,7 @@
         <v>0.68911824325380333</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>9</v>
       </c>
@@ -4993,7 +5005,7 @@
         <v>1.2920967061008812</v>
       </c>
     </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>9</v>
       </c>
@@ -5034,7 +5046,7 @@
         <v>0.17227956081345083</v>
       </c>
     </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>9</v>
       </c>
@@ -5075,7 +5087,7 @@
         <v>0.13485871053317991</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>9</v>
       </c>
@@ -5116,7 +5128,7 @@
         <v>6.1093746356736854E-3</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>9</v>
       </c>
@@ -5157,7 +5169,7 @@
         <v>1.1965200747161964</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>9</v>
       </c>
@@ -5198,7 +5210,7 @@
         <v>0.10787865241732354</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>9</v>
       </c>
@@ -5239,7 +5251,7 @@
         <v>2.2482421642235728E-3</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>9</v>
       </c>
@@ -5280,7 +5292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>9</v>
       </c>
@@ -5321,7 +5333,7 @@
         <v>0.20624177562849991</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>9</v>
       </c>
@@ -5362,7 +5374,7 @@
         <v>0.37498504659727255</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
         <v>9</v>
       </c>
@@ -5403,7 +5415,7 @@
         <v>4.3748255436348464E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>9</v>
       </c>
@@ -5444,7 +5456,7 @@
         <v>0.8635951998184207</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
         <v>9</v>
       </c>
@@ -5485,7 +5497,7 @@
         <v>3.9122623880955193E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
         <v>9</v>
       </c>
@@ -5526,7 +5538,7 @@
         <v>3.3131396681121124</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>9</v>
       </c>
@@ -5567,7 +5579,7 @@
         <v>0.29871378693841744</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
         <v>9</v>
       </c>
@@ -5608,7 +5620,7 @@
         <v>5.5583363127160055E-3</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>9</v>
       </c>
@@ -5649,7 +5661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
         <v>9</v>
       </c>
@@ -5690,7 +5702,7 @@
         <v>0.46825639782769962</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
         <v>9</v>
       </c>
@@ -5731,7 +5743,7 @@
         <v>0.82633481969594036</v>
       </c>
     </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
         <v>9</v>
       </c>
@@ -5772,7 +5784,7 @@
         <v>8.2633481969594039E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
         <v>9</v>
       </c>
@@ -5782,6 +5794,9 @@
       <c r="C128" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D128" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E128" s="6" t="s">
         <v>15</v>
       </c>
@@ -5810,7 +5825,7 @@
         <v>0.77033251450225737</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
         <v>9</v>
       </c>
@@ -5820,6 +5835,9 @@
       <c r="C129" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D129" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E129" s="6" t="s">
         <v>16</v>
       </c>
@@ -5848,7 +5866,7 @@
         <v>3.4897634023995233E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
         <v>9</v>
       </c>
@@ -5858,6 +5876,9 @@
       <c r="C130" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D130" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E130" s="6" t="s">
         <v>17</v>
       </c>
@@ -5886,7 +5907,7 @@
         <v>3.3005074004820987</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
         <v>9</v>
       </c>
@@ -5896,6 +5917,9 @@
       <c r="C131" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D131" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E131" s="6" t="s">
         <v>18</v>
       </c>
@@ -5924,7 +5948,7 @@
         <v>0.29757485743970086</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
         <v>9</v>
       </c>
@@ -5934,6 +5958,9 @@
       <c r="C132" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D132" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E132" s="6" t="s">
         <v>19</v>
       </c>
@@ -5962,7 +5989,7 @@
         <v>5.5452270289596001E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>9</v>
       </c>
@@ -5972,6 +5999,9 @@
       <c r="C133" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D133" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E133" s="6" t="s">
         <v>20</v>
       </c>
@@ -6000,7 +6030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>9</v>
       </c>
@@ -6010,6 +6040,9 @@
       <c r="C134" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D134" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E134" s="6" t="s">
         <v>12</v>
       </c>
@@ -6038,7 +6071,7 @@
         <v>0.40904892586832847</v>
       </c>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>9</v>
       </c>
@@ -6048,6 +6081,9 @@
       <c r="C135" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D135" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E135" s="6" t="s">
         <v>13</v>
       </c>
@@ -6076,7 +6112,7 @@
         <v>0.72185104564999136</v>
       </c>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>9</v>
       </c>
@@ -6086,6 +6122,9 @@
       <c r="C136" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D136" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E136" s="6" t="s">
         <v>14</v>
       </c>
@@ -6114,12 +6153,12 @@
         <v>7.2185104564999131E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>0</v>
@@ -6155,12 +6194,12 @@
         <v>7.1037043832782487</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>0</v>
@@ -6196,12 +6235,12 @@
         <v>1.8983521205815821</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>0</v>
@@ -6237,12 +6276,12 @@
         <v>2.4467782580387611</v>
       </c>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C140" s="4" t="s">
         <v>0</v>
@@ -6278,12 +6317,12 @@
         <v>4.7485776131604203</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C141" s="4" t="s">
         <v>0</v>
@@ -6319,12 +6358,12 @@
         <v>0.22657119081383442</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C142" s="4" t="s">
         <v>0</v>
@@ -6360,12 +6399,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C143" s="4" t="s">
         <v>0</v>
@@ -6401,12 +6440,12 @@
         <v>10.6177747782429</v>
       </c>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C144" s="4" t="s">
         <v>0</v>
@@ -6442,12 +6481,12 @@
         <v>24.50255718056054</v>
       </c>
     </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>0</v>
@@ -6483,12 +6522,12 @@
         <v>5.717263342130793</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>1</v>
@@ -6524,12 +6563,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>1</v>
@@ -6565,12 +6604,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C148" s="4" t="s">
         <v>1</v>
@@ -6606,12 +6645,12 @@
         <v>2.5383061375186982</v>
       </c>
     </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>1</v>
@@ -6647,12 +6686,12 @@
         <v>4.9262100725181615</v>
       </c>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>1</v>
@@ -6688,12 +6727,12 @@
         <v>8.7703975616481522E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>1</v>
@@ -6729,12 +6768,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>1</v>
@@ -6770,12 +6809,12 @@
         <v>3.7093065529581288</v>
       </c>
     </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>1</v>
@@ -6811,12 +6850,12 @@
         <v>8.2429034510180621</v>
       </c>
     </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C154" s="4" t="s">
         <v>1</v>
@@ -6852,12 +6891,12 @@
         <v>1.785962414387247</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C155" s="4" t="s">
         <v>21</v>
@@ -6893,12 +6932,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C156" s="4" t="s">
         <v>21</v>
@@ -6934,12 +6973,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C157" s="4" t="s">
         <v>21</v>
@@ -6975,12 +7014,12 @@
         <v>0.9569189509583762</v>
       </c>
     </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C158" s="4" t="s">
         <v>21</v>
@@ -7016,12 +7055,12 @@
         <v>1.8571376025599435</v>
       </c>
     </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C159" s="4" t="s">
         <v>21</v>
@@ -7057,12 +7096,12 @@
         <v>3.3063622666036394E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C160" s="4" t="s">
         <v>21</v>
@@ -7098,12 +7137,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C161" s="4" t="s">
         <v>21</v>
@@ -7139,12 +7178,12 @@
         <v>1.4047739167464559</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C162" s="4" t="s">
         <v>21</v>
@@ -7180,12 +7219,12 @@
         <v>3.2417859617225901</v>
       </c>
     </row>
-    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C163" s="4" t="s">
         <v>21</v>
@@ -7221,12 +7260,12 @@
         <v>0.75641672440193786</v>
       </c>
     </row>
-    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C164" s="4" t="s">
         <v>2</v>
@@ -7262,12 +7301,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C165" s="4" t="s">
         <v>2</v>
@@ -7303,12 +7342,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C166" s="4" t="s">
         <v>2</v>
@@ -7344,12 +7383,12 @@
         <v>6.5819609155682288</v>
       </c>
     </row>
-    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C167" s="4" t="s">
         <v>2</v>
@@ -7385,12 +7424,12 @@
         <v>12.773921033374256</v>
       </c>
     </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C168" s="4" t="s">
         <v>2</v>
@@ -7426,12 +7465,12 @@
         <v>0.19046509394942093</v>
       </c>
     </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C169" s="4" t="s">
         <v>2</v>
@@ -7467,12 +7506,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C170" s="4" t="s">
         <v>2</v>
@@ -7508,12 +7547,12 @@
         <v>9.4558477909893739</v>
       </c>
     </row>
-    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C171" s="4" t="s">
         <v>2</v>
@@ -7549,12 +7588,12 @@
         <v>17.729714608105073</v>
       </c>
     </row>
-    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C172" s="4" t="s">
         <v>2</v>
@@ -7590,12 +7629,12 @@
         <v>2.3639619477473435</v>
       </c>
     </row>
-    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C173" s="4" t="s">
         <v>22</v>
@@ -7631,12 +7670,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C174" s="4" t="s">
         <v>22</v>
@@ -7672,12 +7711,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C175" s="4" t="s">
         <v>22</v>
@@ -7713,12 +7752,12 @@
         <v>0.80665030878663668</v>
       </c>
     </row>
-    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C176" s="4" t="s">
         <v>22</v>
@@ -7754,12 +7793,12 @@
         <v>1.5655041830490561</v>
       </c>
     </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C177" s="4" t="s">
         <v>22</v>
@@ -7795,12 +7834,12 @@
         <v>2.5612665445521154E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B178" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C178" s="4" t="s">
         <v>22</v>
@@ -7836,12 +7875,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B179" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C179" s="4" t="s">
         <v>22</v>
@@ -7877,12 +7916,12 @@
         <v>1.2565470476883773</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C180" s="4" t="s">
         <v>22</v>
@@ -7918,12 +7957,12 @@
         <v>2.217435966508901</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>22</v>
@@ -7959,12 +7998,12 @@
         <v>0.22174359665089008</v>
       </c>
     </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>3</v>
@@ -8000,12 +8039,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>3</v>
@@ -8041,12 +8080,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>3</v>
@@ -8082,12 +8121,12 @@
         <v>0.42243636683047919</v>
       </c>
     </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>3</v>
@@ -8123,12 +8162,12 @@
         <v>0.81984212011265079</v>
       </c>
     </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>3</v>
@@ -8164,12 +8203,12 @@
         <v>1.0865979279918064E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>3</v>
@@ -8205,12 +8244,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>3</v>
@@ -8246,12 +8285,12 @@
         <v>0.42881077211534074</v>
       </c>
     </row>
-    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C189" s="4" t="s">
         <v>3</v>
@@ -8287,12 +8326,12 @@
         <v>0.98956332026617089</v>
       </c>
     </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C190" s="4" t="s">
         <v>3</v>
@@ -8328,12 +8367,12 @@
         <v>0.23089810806210656</v>
       </c>
     </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C191" s="4" t="s">
         <v>23</v>
@@ -8369,12 +8408,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C192" s="4" t="s">
         <v>23</v>
@@ -8410,12 +8449,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B193" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C193" s="4" t="s">
         <v>23</v>
@@ -8451,12 +8490,12 @@
         <v>1.4218001146465848</v>
       </c>
     </row>
-    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B194" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C194" s="4" t="s">
         <v>23</v>
@@ -8492,12 +8531,12 @@
         <v>2.7593543356934376</v>
       </c>
     </row>
-    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B195" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C195" s="4" t="s">
         <v>23</v>
@@ -8533,12 +8572,12 @@
         <v>3.6571781690695658E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C196" s="4" t="s">
         <v>23</v>
@@ -8574,12 +8613,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C197" s="4" t="s">
         <v>23</v>
@@ -8615,12 +8654,12 @@
         <v>1.8212246857339311</v>
       </c>
     </row>
-    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C198" s="4" t="s">
         <v>23</v>
@@ -8656,12 +8695,12 @@
         <v>3.2139259160010547</v>
       </c>
     </row>
-    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C199" s="4" t="s">
         <v>23</v>
@@ -8697,12 +8736,12 @@
         <v>0.32139259160010547</v>
       </c>
     </row>
-    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C200" s="4" t="s">
         <v>27</v>
@@ -8738,12 +8777,12 @@
         <v>0.22492766813538143</v>
       </c>
     </row>
-    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C201" s="4" t="s">
         <v>27</v>
@@ -8779,12 +8818,12 @@
         <v>6.010834527227632E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B202" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C202" s="4" t="s">
         <v>27</v>
@@ -8820,12 +8859,12 @@
         <v>1.5869555139184914</v>
       </c>
     </row>
-    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C203" s="4" t="s">
         <v>27</v>
@@ -8861,12 +8900,12 @@
         <v>3.079879184685586</v>
       </c>
     </row>
-    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B204" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C204" s="4" t="s">
         <v>27</v>
@@ -8902,12 +8941,12 @@
         <v>4.1042356023004808E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C205" s="4" t="s">
         <v>27</v>
@@ -8943,12 +8982,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C206" s="4" t="s">
         <v>27</v>
@@ -8984,12 +9023,12 @@
         <v>1.5661759356443015</v>
       </c>
     </row>
-    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C207" s="4" t="s">
         <v>27</v>
@@ -9025,12 +9064,12 @@
         <v>3.6142521591791565</v>
       </c>
     </row>
-    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C208" s="4" t="s">
         <v>27</v>
@@ -9066,12 +9105,12 @@
         <v>0.84332550380847005</v>
       </c>
     </row>
-    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C209" s="4" t="s">
         <v>4</v>
@@ -9107,12 +9146,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B210" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C210" s="4" t="s">
         <v>4</v>
@@ -9148,12 +9187,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C211" s="4" t="s">
         <v>4</v>
@@ -9189,12 +9228,12 @@
         <v>3.5472585203279388</v>
       </c>
     </row>
-    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>4</v>
@@ -9230,12 +9269,12 @@
         <v>6.8843314028888036</v>
       </c>
     </row>
-    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>4</v>
@@ -9271,12 +9310,12 @@
         <v>9.1243180296226259E-2</v>
       </c>
     </row>
-    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C214" s="4" t="s">
         <v>4</v>
@@ -9312,12 +9351,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C215" s="4" t="s">
         <v>4</v>
@@ -9353,12 +9392,12 @@
         <v>3.3629822751325134</v>
       </c>
     </row>
-    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>4</v>
@@ -9394,12 +9433,12 @@
         <v>7.7607283272288772</v>
       </c>
     </row>
-    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B217" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>4</v>
@@ -9435,12 +9474,12 @@
         <v>1.8108366096867381</v>
       </c>
     </row>
-    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B218" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>5</v>
@@ -9476,12 +9515,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B219" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C219" s="4" t="s">
         <v>5</v>
@@ -9517,12 +9556,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B220" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>5</v>
@@ -9558,12 +9597,12 @@
         <v>0.4102496823316541</v>
       </c>
     </row>
-    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B221" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>5</v>
@@ -9599,12 +9638,12 @@
         <v>0.79619084848652655</v>
       </c>
     </row>
-    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C222" s="4" t="s">
         <v>5</v>
@@ -9640,12 +9679,12 @@
         <v>2.3563652209879462E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>5</v>
@@ -9681,12 +9720,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B224" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>5</v>
@@ -9722,12 +9761,12 @@
         <v>0.27057947148381012</v>
       </c>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>5</v>
@@ -9763,12 +9802,12 @@
         <v>0.62441416496263868</v>
       </c>
     </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B226" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>5</v>
@@ -9804,12 +9843,12 @@
         <v>0.14569663849128237</v>
       </c>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B227" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>24</v>
@@ -9845,12 +9884,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>24</v>
@@ -9886,12 +9925,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>24</v>
@@ -9927,12 +9966,12 @@
         <v>5.5326707346212936E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>24</v>
@@ -9968,12 +10007,12 @@
         <v>0.10737514241470054</v>
       </c>
     </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>24</v>
@@ -10009,12 +10048,12 @@
         <v>3.1666568187189788E-3</v>
       </c>
     </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>24</v>
@@ -10050,12 +10089,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>24</v>
@@ -10091,12 +10130,12 @@
         <v>9.9164677016776767E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>24</v>
@@ -10132,12 +10171,12 @@
         <v>0.2288415623464079</v>
       </c>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>24</v>
@@ -10173,12 +10212,12 @@
         <v>5.339636454749519E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C236" s="4" t="s">
         <v>6</v>
@@ -10214,12 +10253,12 @@
         <v>0.87238901802043411</v>
       </c>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>6</v>
@@ -10255,12 +10294,12 @@
         <v>0.23313210305169121</v>
       </c>
     </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B238" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>6</v>
@@ -10296,12 +10335,12 @@
         <v>3.6057961311601612</v>
       </c>
     </row>
-    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>6</v>
@@ -10337,12 +10376,12 @@
         <v>6.9979380966758402</v>
       </c>
     </row>
-    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>6</v>
@@ -10378,12 +10417,12 @@
         <v>0.11129867348144647</v>
       </c>
     </row>
-    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C241" s="4" t="s">
         <v>6</v>
@@ -10419,12 +10458,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>6</v>
@@ -10460,12 +10499,12 @@
         <v>5.5177105628534688</v>
       </c>
     </row>
-    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>6</v>
@@ -10501,12 +10540,12 @@
         <v>10.345707305350253</v>
       </c>
     </row>
-    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>6</v>
@@ -10542,12 +10581,12 @@
         <v>1.3794276407133672</v>
       </c>
     </row>
-    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>7</v>
@@ -10583,12 +10622,12 @@
         <v>9.0767392948848558E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B246" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>7</v>
@@ -10624,12 +10663,12 @@
         <v>2.4256143497428412E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>7</v>
@@ -10665,12 +10704,12 @@
         <v>0.75032745156080383</v>
       </c>
     </row>
-    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B248" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>7</v>
@@ -10706,12 +10745,12 @@
         <v>1.4561957657238995</v>
       </c>
     </row>
-    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B249" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>7</v>
@@ -10747,12 +10786,12 @@
         <v>3.4740088040652324E-2</v>
       </c>
     </row>
-    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B250" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>7</v>
@@ -10788,12 +10827,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>7</v>
@@ -10829,12 +10868,12 @@
         <v>2.040380085817838</v>
       </c>
     </row>
-    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C252" s="4" t="s">
         <v>7</v>
@@ -10870,12 +10909,12 @@
         <v>3.709781974214251</v>
       </c>
     </row>
-    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>7</v>
@@ -10911,12 +10950,12 @@
         <v>0.43280789699166267</v>
       </c>
     </row>
-    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>8</v>
@@ -10952,12 +10991,12 @@
         <v>0.32901902991500126</v>
       </c>
     </row>
-    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>8</v>
@@ -10993,12 +11032,12 @@
         <v>8.7925107725639523E-2</v>
       </c>
     </row>
-    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>8</v>
@@ -11034,12 +11073,12 @@
         <v>1.176062845256054</v>
       </c>
     </row>
-    <row r="257" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>8</v>
@@ -11075,12 +11114,12 @@
         <v>2.2824404623936196</v>
       </c>
     </row>
-    <row r="258" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B258" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C258" s="4" t="s">
         <v>8</v>
@@ -11116,12 +11155,12 @@
         <v>4.8617495863861972E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>8</v>
@@ -11157,12 +11196,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C260" s="4" t="s">
         <v>8</v>
@@ -11198,12 +11237,12 @@
         <v>2.7052517202899047</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C261" s="4" t="s">
         <v>8</v>
@@ -11239,12 +11278,12 @@
         <v>4.773973624041008</v>
       </c>
     </row>
-    <row r="262" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B262" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>8</v>
@@ -11280,16 +11319,19 @@
         <v>0.89099037456254992</v>
       </c>
     </row>
-    <row r="263" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C263" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D263" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E263" s="6" t="s">
         <v>15</v>
       </c>
@@ -11318,16 +11360,19 @@
         <v>0.52223689953621089</v>
       </c>
     </row>
-    <row r="264" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C264" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D264" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E264" s="6" t="s">
         <v>16</v>
       </c>
@@ -11356,16 +11401,19 @@
         <v>0.13955951320471557</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C265" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D265" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E265" s="6" t="s">
         <v>17</v>
       </c>
@@ -11394,16 +11442,19 @@
         <v>2.0847309967095096</v>
       </c>
     </row>
-    <row r="266" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C266" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D266" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E266" s="6" t="s">
         <v>18</v>
       </c>
@@ -11432,16 +11483,19 @@
         <v>4.0459354695964285</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C267" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D267" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E267" s="6" t="s">
         <v>19</v>
       </c>
@@ -11470,16 +11524,19 @@
         <v>8.6306921137634926E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C268" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D268" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E268" s="6" t="s">
         <v>20</v>
       </c>
@@ -11508,16 +11565,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C269" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D269" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E269" s="6" t="s">
         <v>12</v>
       </c>
@@ -11546,16 +11606,19 @@
         <v>5.04894545585445</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C270" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D270" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E270" s="6" t="s">
         <v>13</v>
       </c>
@@ -11584,15 +11647,18 @@
         <v>8.909903745625499</v>
       </c>
     </row>
-    <row r="271" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C271" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="D271" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="E271" s="6" t="s">
         <v>14</v>
@@ -11632,6 +11698,9 @@
       <c r="C272" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="D272" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E272" s="6" t="s">
         <v>15</v>
       </c>
@@ -16836,6 +16905,9 @@
       <c r="C399" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D399" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E399" s="6" t="s">
         <v>16</v>
       </c>
@@ -16874,6 +16946,9 @@
       <c r="C400" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D400" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E400" s="6" t="s">
         <v>17</v>
       </c>
@@ -16912,6 +16987,9 @@
       <c r="C401" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D401" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E401" s="6" t="s">
         <v>18</v>
       </c>
@@ -16950,6 +17028,9 @@
       <c r="C402" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D402" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E402" s="6" t="s">
         <v>19</v>
       </c>
@@ -16988,6 +17069,9 @@
       <c r="C403" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D403" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E403" s="6" t="s">
         <v>20</v>
       </c>
@@ -17026,6 +17110,9 @@
       <c r="C404" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D404" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E404" s="6" t="s">
         <v>12</v>
       </c>
@@ -17064,6 +17151,9 @@
       <c r="C405" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D405" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E405" s="6" t="s">
         <v>13</v>
       </c>
@@ -17102,6 +17192,9 @@
       <c r="C406" s="4" t="s">
         <v>25</v>
       </c>
+      <c r="D406" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="E406" s="6" t="s">
         <v>14</v>
       </c>
@@ -17131,7 +17224,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M406" xr:uid="{AEF4BDD2-5D39-4ECE-8BF4-156E73BF5FC9}"/>
+  <autoFilter ref="A1:M406" xr:uid="{AEF4BDD2-5D39-4ECE-8BF4-156E73BF5FC9}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SSP2 - PkBudg500"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>